<commit_message>
Site Ready For Kevin's mailing tomorrow
</commit_message>
<xml_diff>
--- a/UConnBleedBlue/wwwroot/Data/Players.xlsx
+++ b/UConnBleedBlue/wwwroot/Data/Players.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\UConnBleedBlue\UConnBleedBlue\wwwroot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F1D126-8BD7-4E59-8506-D19B7F518955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCB1935-554E-4436-B000-260478DAB933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2325" windowWidth="38640" windowHeight="21120" xr2:uid="{4F83266A-41F9-4FA3-9290-1EB5622BBFC1}"/>
   </bookViews>
@@ -1931,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F97E2D-D2EE-4E19-AA28-ED70E4256082}">
   <dimension ref="A1:G244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E229" sqref="E229"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="Q166" sqref="Q166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2322,7 @@
         <v>132</v>
       </c>
       <c r="E23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
@@ -3000,7 +3000,7 @@
         <v>133</v>
       </c>
       <c r="E70" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -3225,7 +3225,7 @@
         <v>440</v>
       </c>
       <c r="E85" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3257,8 +3257,14 @@
       <c r="B88" s="3" t="s">
         <v>336</v>
       </c>
+      <c r="C88" s="1">
+        <v>1971</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E88" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,7 +3707,7 @@
         <v>129</v>
       </c>
       <c r="E119" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119" s="1">
         <v>2</v>
@@ -3725,8 +3731,11 @@
       <c r="B121" s="3" t="s">
         <v>272</v>
       </c>
+      <c r="C121" s="1">
+        <v>1978</v>
+      </c>
       <c r="E121" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4034,7 +4043,7 @@
         <v>129</v>
       </c>
       <c r="E143" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G143" s="1">
         <v>2</v>
@@ -4388,8 +4397,11 @@
       <c r="B166" s="3" t="s">
         <v>357</v>
       </c>
+      <c r="C166" s="1">
+        <v>1970</v>
+      </c>
       <c r="E166" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4399,8 +4411,11 @@
       <c r="B167" s="3" t="s">
         <v>418</v>
       </c>
+      <c r="C167" s="1">
+        <v>1975</v>
+      </c>
       <c r="E167" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -4544,14 +4559,14 @@
       <c r="B178" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>153</v>
+      <c r="C178" s="1">
+        <v>2007</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E178" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G178" s="1">
         <v>2</v>
@@ -4619,7 +4634,7 @@
         <v>131</v>
       </c>
       <c r="E182" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G182" s="1">
         <v>2</v>
@@ -4639,7 +4654,7 @@
         <v>133</v>
       </c>
       <c r="E183" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G183" s="1">
         <v>2</v>
@@ -4714,13 +4729,13 @@
         <v>36</v>
       </c>
       <c r="C189" s="1">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E189" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G189" s="1">
         <v>2</v>

</xml_diff>